<commit_message>
Start going through Alt1
</commit_message>
<xml_diff>
--- a/CH-177 Table Transformation.xlsx
+++ b/CH-177 Table Transformation.xlsx
@@ -8,13 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2721CA1F-2862-4A51-AD78-BCAFA207D4A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B1F96A1-1FAC-445D-BB70-6B1E9E900415}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
+    <sheet name="Alt1" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_a">'Alt1'!$C$3:$C$24</definedName>
+    <definedName name="_b">'Alt1'!$B$3:$B$24</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Alt1'!$I$16:$M$37</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -35,8 +41,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="10">
   <si>
     <t>Result</t>
   </si>
@@ -72,7 +100,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -113,6 +141,14 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Tw Cen MT"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="7">
@@ -342,10 +378,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -450,8 +487,13 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -889,12 +931,39 @@
 </a:theme>
 </file>
 
+<file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
+<wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
+  <wetp:taskpane dockstate="right" visibility="0" width="771" row="8">
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+  </wetp:taskpane>
+</wetp:taskpanes>
+</file>
+
+<file path=xl/webextensions/webextension1.xml><?xml version="1.0" encoding="utf-8"?>
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{90A67CF5-9406-4620-8641-2CECA7CB2482}">
+  <we:reference id="wa200003696" version="1.3.0.0" store="en-US" storeType="OMEX"/>
+  <we:alternateReferences>
+    <we:reference id="wa200003696" version="1.3.0.0" store="" storeType="OMEX"/>
+  </we:alternateReferences>
+  <we:properties/>
+  <we:bindings/>
+  <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+  <we:extLst>
+    <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{7C84B067-C214-45C3-A712-C9D94CD141B2}">
+      <we:customFunctionIdList>
+        <we:customFunctionIds>_xldudf_LABS_GENERATIVEAI</we:customFunctionIds>
+      </we:customFunctionIdList>
+    </a:ext>
+  </we:extLst>
+</we:webextension>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:J24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16:C19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -915,7 +984,7 @@
       </c>
       <c r="F1" s="35"/>
       <c r="G1" s="35"/>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="36" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1152,9 +1221,765 @@
     <mergeCell ref="E1:G1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="J1" r:id="rId1" xr:uid="{453801F0-6A53-4987-9EBF-04092339F896}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <drawing r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28BDC360-8D84-479A-A154-556548DB1B28}">
+  <dimension ref="B1:K37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2.8984375" customWidth="1"/>
+    <col min="3" max="3" width="12.3984375" style="5" customWidth="1"/>
+    <col min="4" max="4" width="10.5" style="9" customWidth="1"/>
+    <col min="5" max="7" width="10.5" style="5" customWidth="1"/>
+    <col min="10" max="10" width="10.09765625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:11" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="4"/>
+      <c r="E1" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="J1" s="36" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="2:11" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="1"/>
+      <c r="C2" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="4"/>
+      <c r="E2" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="21" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" cm="1">
+        <f t="array" ref="B3:B24">ROW(C3:C24)</f>
+        <v>3</v>
+      </c>
+      <c r="C3" s="13" cm="1">
+        <f t="array" aca="1" ref="C3" ca="1">C3:C24&gt;""</f>
+        <v>0</v>
+      </c>
+      <c r="D3" s="5"/>
+      <c r="E3" s="13">
+        <v>45493</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" s="15">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="1">
+        <v>4</v>
+      </c>
+      <c r="C4" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="5"/>
+      <c r="E4" s="11">
+        <v>45509</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" s="7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="1">
+        <v>5</v>
+      </c>
+      <c r="C5" s="24">
+        <v>10</v>
+      </c>
+      <c r="D5" s="5"/>
+      <c r="E5" s="11">
+        <v>45509</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5" s="7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="1">
+        <v>6</v>
+      </c>
+      <c r="C6" s="25">
+        <v>45509</v>
+      </c>
+      <c r="D6" s="5"/>
+      <c r="E6" s="11">
+        <v>45509</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="G6" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="1">
+        <v>7</v>
+      </c>
+      <c r="C7" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="5"/>
+      <c r="E7" s="32">
+        <v>45517</v>
+      </c>
+      <c r="F7" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="G7" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="1">
+        <v>8</v>
+      </c>
+      <c r="C8" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="5"/>
+      <c r="E8" s="16">
+        <v>45553</v>
+      </c>
+      <c r="F8" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="G8" s="18">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="1">
+        <v>9</v>
+      </c>
+      <c r="C9" s="26">
+        <v>8</v>
+      </c>
+      <c r="D9" s="5"/>
+      <c r="E9" s="16">
+        <v>45553</v>
+      </c>
+      <c r="F9" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="G9" s="18">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="1">
+        <v>10</v>
+      </c>
+      <c r="C10" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="5"/>
+      <c r="E10" s="16">
+        <v>45553</v>
+      </c>
+      <c r="F10" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="G10" s="18">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="1">
+        <v>11</v>
+      </c>
+      <c r="C11" s="26">
+        <v>2</v>
+      </c>
+      <c r="D11" s="5"/>
+      <c r="E11" s="11">
+        <v>45566</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="G11" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B12" s="1">
+        <v>12</v>
+      </c>
+      <c r="C12" s="30">
+        <v>45517</v>
+      </c>
+      <c r="E12" s="12">
+        <v>45566</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G12" s="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B13" s="1">
+        <v>13</v>
+      </c>
+      <c r="C13" s="30" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B14" s="1">
+        <v>14</v>
+      </c>
+      <c r="C14" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B15" s="1">
+        <v>15</v>
+      </c>
+      <c r="C15" s="27">
+        <v>45553</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B16" s="1">
+        <v>16</v>
+      </c>
+      <c r="C16" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="E16" s="5" cm="1">
+        <f t="array" aca="1" ref="E16:G25" ca="1">_xlfn.LET(
+    _xlpm.a, C3:C24,
+    _xlpm.b, ROW(_xlpm.a),
+    _xlfn._xlws.FILTER(
+        _xlfn.HSTACK(_xlfn.SCAN(, _xlpm.a, _xleta.MAX), _xlpm.a, _xlfn.XLOOKUP(_xlpm.b, _xlpm.b / (_xlpm.a &lt; 99), _xlpm.a, , 1)),
+        _xlpm.a &gt; ""
+    )
+)</f>
+        <v>45493</v>
+      </c>
+      <c r="F16" s="5" t="str">
+        <f ca="1"/>
+        <v>A</v>
+      </c>
+      <c r="G16" s="5">
+        <f ca="1"/>
+        <v>10</v>
+      </c>
+      <c r="I16" cm="1">
+        <f t="array" aca="1" ref="I16:I37" ca="1">_xlfn.SCAN(, C3:C24, _xleta.MAX)</f>
+        <v>45493</v>
+      </c>
+      <c r="J16" s="37" cm="1">
+        <f t="array" aca="1" ref="J16:J37" ca="1">C3:C24</f>
+        <v>45493</v>
+      </c>
+      <c r="K16" cm="1">
+        <f t="array" aca="1" ref="K16" ca="1">_xlfn.XLOOKUP(B3, _b / (_a &lt; 99), _a, , 1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B17" s="1">
+        <v>17</v>
+      </c>
+      <c r="C17" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="E17" s="5">
+        <f ca="1"/>
+        <v>45509</v>
+      </c>
+      <c r="F17" s="5" t="str">
+        <f ca="1"/>
+        <v>C</v>
+      </c>
+      <c r="G17" s="5">
+        <f ca="1"/>
+        <v>8</v>
+      </c>
+      <c r="I17">
+        <f ca="1"/>
+        <v>45493</v>
+      </c>
+      <c r="J17" t="str">
+        <f ca="1"/>
+        <v>A</v>
+      </c>
+      <c r="K17" cm="1">
+        <f t="array" aca="1" ref="K17" ca="1">_xlfn.XLOOKUP(B4, _b / (_a &lt; 99), _a, , 1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B18" s="1">
+        <v>18</v>
+      </c>
+      <c r="C18" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="E18" s="5">
+        <f ca="1"/>
+        <v>45509</v>
+      </c>
+      <c r="F18" s="5" t="str">
+        <f ca="1"/>
+        <v>B</v>
+      </c>
+      <c r="G18" s="5">
+        <f ca="1"/>
+        <v>8</v>
+      </c>
+      <c r="I18">
+        <f ca="1"/>
+        <v>45493</v>
+      </c>
+      <c r="J18">
+        <f ca="1"/>
+        <v>10</v>
+      </c>
+      <c r="K18" cm="1">
+        <f t="array" aca="1" ref="K18" ca="1">_xlfn.XLOOKUP(B5, _b / (_a &lt; 99), _a, , 1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B19" s="1">
+        <v>19</v>
+      </c>
+      <c r="C19" s="28">
+        <v>5</v>
+      </c>
+      <c r="E19" s="5">
+        <f ca="1"/>
+        <v>45509</v>
+      </c>
+      <c r="F19" s="5" t="str">
+        <f ca="1"/>
+        <v>A</v>
+      </c>
+      <c r="G19" s="5">
+        <f ca="1"/>
+        <v>2</v>
+      </c>
+      <c r="I19">
+        <f ca="1"/>
+        <v>45509</v>
+      </c>
+      <c r="J19">
+        <f ca="1"/>
+        <v>45509</v>
+      </c>
+      <c r="K19" cm="1">
+        <f t="array" aca="1" ref="K19" ca="1">_xlfn.XLOOKUP(B6, _b / (_a &lt; 99), _a, , 1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B20" s="1">
+        <v>20</v>
+      </c>
+      <c r="C20" s="25">
+        <v>45566</v>
+      </c>
+      <c r="E20" s="5">
+        <f ca="1"/>
+        <v>45517</v>
+      </c>
+      <c r="F20" s="5" t="str">
+        <f ca="1"/>
+        <v>B</v>
+      </c>
+      <c r="G20" s="5">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="I20">
+        <f ca="1"/>
+        <v>45509</v>
+      </c>
+      <c r="J20" t="str">
+        <f ca="1"/>
+        <v>C</v>
+      </c>
+      <c r="K20" cm="1">
+        <f t="array" aca="1" ref="K20" ca="1">_xlfn.XLOOKUP(B7, _b / (_a &lt; 99), _a, , 1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B21" s="1">
+        <v>21</v>
+      </c>
+      <c r="C21" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="E21" s="5">
+        <f ca="1"/>
+        <v>45553</v>
+      </c>
+      <c r="F21" s="5" t="str">
+        <f ca="1"/>
+        <v>A</v>
+      </c>
+      <c r="G21" s="5">
+        <f ca="1"/>
+        <v>5</v>
+      </c>
+      <c r="I21">
+        <f ca="1"/>
+        <v>45509</v>
+      </c>
+      <c r="J21" t="str">
+        <f ca="1"/>
+        <v>B</v>
+      </c>
+      <c r="K21" cm="1">
+        <f t="array" aca="1" ref="K21" ca="1">_xlfn.XLOOKUP(B8, _b / (_a &lt; 99), _a, , 1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B22" s="1">
+        <v>22</v>
+      </c>
+      <c r="C22" s="26">
+        <v>1</v>
+      </c>
+      <c r="E22" s="5">
+        <f ca="1"/>
+        <v>45553</v>
+      </c>
+      <c r="F22" s="5" t="str">
+        <f ca="1"/>
+        <v>B</v>
+      </c>
+      <c r="G22" s="5">
+        <f ca="1"/>
+        <v>5</v>
+      </c>
+      <c r="I22">
+        <f ca="1"/>
+        <v>45509</v>
+      </c>
+      <c r="J22">
+        <f ca="1"/>
+        <v>8</v>
+      </c>
+      <c r="K22" cm="1">
+        <f t="array" aca="1" ref="K22" ca="1">_xlfn.XLOOKUP(B9, _b / (_a &lt; 99), _a, , 1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B23" s="1">
+        <v>23</v>
+      </c>
+      <c r="C23" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="E23" s="5">
+        <f ca="1"/>
+        <v>45553</v>
+      </c>
+      <c r="F23" s="5" t="str">
+        <f ca="1"/>
+        <v>C</v>
+      </c>
+      <c r="G23" s="5">
+        <f ca="1"/>
+        <v>5</v>
+      </c>
+      <c r="I23">
+        <f ca="1"/>
+        <v>45509</v>
+      </c>
+      <c r="J23" t="str">
+        <f ca="1"/>
+        <v>A</v>
+      </c>
+      <c r="K23" cm="1">
+        <f t="array" aca="1" ref="K23" ca="1">_xlfn.XLOOKUP(B10, _b / (_a &lt; 99), _a, , 1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B24" s="1">
+        <v>24</v>
+      </c>
+      <c r="C24" s="29">
+        <v>2</v>
+      </c>
+      <c r="E24" s="5">
+        <f ca="1"/>
+        <v>45566</v>
+      </c>
+      <c r="F24" s="5" t="str">
+        <f ca="1"/>
+        <v>A</v>
+      </c>
+      <c r="G24" s="5">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="I24">
+        <f ca="1"/>
+        <v>45509</v>
+      </c>
+      <c r="J24">
+        <f ca="1"/>
+        <v>2</v>
+      </c>
+      <c r="K24" cm="1">
+        <f t="array" aca="1" ref="K24" ca="1">_xlfn.XLOOKUP(B11, _b / (_a &lt; 99), _a, , 1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="E25" s="5">
+        <f ca="1"/>
+        <v>45566</v>
+      </c>
+      <c r="F25" s="5" t="str">
+        <f ca="1"/>
+        <v>B</v>
+      </c>
+      <c r="G25" s="5">
+        <f ca="1"/>
+        <v>2</v>
+      </c>
+      <c r="I25">
+        <f ca="1"/>
+        <v>45517</v>
+      </c>
+      <c r="J25">
+        <f ca="1"/>
+        <v>45517</v>
+      </c>
+      <c r="K25" cm="1">
+        <f t="array" aca="1" ref="K25" ca="1">_xlfn.XLOOKUP(B12, _b / (_a &lt; 99), _a, , 1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="I26">
+        <f ca="1"/>
+        <v>45517</v>
+      </c>
+      <c r="J26" t="str">
+        <f ca="1"/>
+        <v>B</v>
+      </c>
+      <c r="K26" cm="1">
+        <f t="array" aca="1" ref="K26" ca="1">_xlfn.XLOOKUP(B13, _b / (_a &lt; 99), _a, , 1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="I27">
+        <f ca="1"/>
+        <v>45517</v>
+      </c>
+      <c r="J27">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="K27" cm="1">
+        <f t="array" aca="1" ref="K27" ca="1">_xlfn.XLOOKUP(B14, _b / (_a &lt; 99), _a, , 1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="I28">
+        <f ca="1"/>
+        <v>45553</v>
+      </c>
+      <c r="J28">
+        <f ca="1"/>
+        <v>45553</v>
+      </c>
+      <c r="K28" cm="1">
+        <f t="array" aca="1" ref="K28" ca="1">_xlfn.XLOOKUP(B15, _b / (_a &lt; 99), _a, , 1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="I29">
+        <f ca="1"/>
+        <v>45553</v>
+      </c>
+      <c r="J29" t="str">
+        <f ca="1"/>
+        <v>A</v>
+      </c>
+      <c r="K29" cm="1">
+        <f t="array" aca="1" ref="K29" ca="1">_xlfn.XLOOKUP(B16, _b / (_a &lt; 99), _a, , 1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="I30">
+        <f ca="1"/>
+        <v>45553</v>
+      </c>
+      <c r="J30" t="str">
+        <f ca="1"/>
+        <v>B</v>
+      </c>
+      <c r="K30" cm="1">
+        <f t="array" aca="1" ref="K30" ca="1">_xlfn.XLOOKUP(B17, _b / (_a &lt; 99), _a, , 1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="I31">
+        <f ca="1"/>
+        <v>45553</v>
+      </c>
+      <c r="J31" t="str">
+        <f ca="1"/>
+        <v>C</v>
+      </c>
+      <c r="K31" cm="1">
+        <f t="array" aca="1" ref="K31" ca="1">_xlfn.XLOOKUP(B18, _b / (_a &lt; 99), _a, , 1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="I32">
+        <f ca="1"/>
+        <v>45553</v>
+      </c>
+      <c r="J32">
+        <f ca="1"/>
+        <v>5</v>
+      </c>
+      <c r="K32" cm="1">
+        <f t="array" aca="1" ref="K32" ca="1">_xlfn.XLOOKUP(B19, _b / (_a &lt; 99), _a, , 1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I33">
+        <f ca="1"/>
+        <v>45566</v>
+      </c>
+      <c r="J33">
+        <f ca="1"/>
+        <v>45566</v>
+      </c>
+      <c r="K33" cm="1">
+        <f t="array" aca="1" ref="K33" ca="1">_xlfn.XLOOKUP(B20, _b / (_a &lt; 99), _a, , 1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I34">
+        <f ca="1"/>
+        <v>45566</v>
+      </c>
+      <c r="J34" t="str">
+        <f ca="1"/>
+        <v>A</v>
+      </c>
+      <c r="K34" cm="1">
+        <f t="array" aca="1" ref="K34" ca="1">_xlfn.XLOOKUP(B21, _b / (_a &lt; 99), _a, , 1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I35">
+        <f ca="1"/>
+        <v>45566</v>
+      </c>
+      <c r="J35">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="K35" cm="1">
+        <f t="array" aca="1" ref="K35" ca="1">_xlfn.XLOOKUP(B22, _b / (_a &lt; 99), _a, , 1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I36">
+        <f ca="1"/>
+        <v>45566</v>
+      </c>
+      <c r="J36" t="str">
+        <f ca="1"/>
+        <v>B</v>
+      </c>
+      <c r="K36" cm="1">
+        <f t="array" aca="1" ref="K36" ca="1">_xlfn.XLOOKUP(B23, _b / (_a &lt; 99), _a, , 1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I37">
+        <f ca="1"/>
+        <v>45566</v>
+      </c>
+      <c r="J37">
+        <f ca="1"/>
+        <v>2</v>
+      </c>
+      <c r="K37" cm="1">
+        <f t="array" aca="1" ref="K37" ca="1">_xlfn.XLOOKUP(B24, _b / (_a &lt; 99), _a, , 1)</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="E1:G1"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="J1" r:id="rId1" xr:uid="{199854B6-B54F-4F68-9670-2D5C85494822}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
I think I found the problem.
</commit_message>
<xml_diff>
--- a/CH-177 Table Transformation.xlsx
+++ b/CH-177 Table Transformation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B1F96A1-1FAC-445D-BB70-6B1E9E900415}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94C21303-2BC5-4B01-8D6C-03675B6D8221}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Alt1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_a">'Alt1'!$C$3:$C$24</definedName>
+    <definedName name="_a11">'Alt1'!$S$6:$S$27</definedName>
     <definedName name="_b">'Alt1'!$B$3:$B$24</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Alt1'!$I$16:$M$37</definedName>
   </definedNames>
@@ -43,8 +43,9 @@
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
 <metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
+  <metadataTypes count="2">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+    <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
   </metadataTypes>
   <futureMetadata name="XLDAPR" count="1">
     <bk>
@@ -55,16 +56,30 @@
       </extLst>
     </bk>
   </futureMetadata>
+  <futureMetadata name="XLRICHVALUE" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
   <cellMetadata count="1">
     <bk>
       <rc t="1" v="0"/>
     </bk>
   </cellMetadata>
+  <valueMetadata count="1">
+    <bk>
+      <rc t="2" v="0"/>
+    </bk>
+  </valueMetadata>
 </metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="10">
   <si>
     <t>Result</t>
   </si>
@@ -484,13 +499,13 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -665,6 +680,68 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
+<rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
+  <global>
+    <keyFlags>
+      <key name="_Self">
+        <flag name="ExcludeFromFile" value="1"/>
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_DisplayString">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Flags">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Format">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_SubLabel">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Attribution">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Icon">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Display">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_CanonicalPropertyNames">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_ClassificationId">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+    </keyFlags>
+  </global>
+</rvTypesInfo>
+</file>
+
+<file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
+  <rv s="0">
+    <v>0</v>
+    <v>8</v>
+    <v>21</v>
+    <v>0</v>
+  </rv>
+</rvData>
+</file>
+
+<file path=xl/richData/rdrichvaluestructure.xml><?xml version="1.0" encoding="utf-8"?>
+<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
+  <s t="_error">
+    <k n="colOffset" t="i"/>
+    <k n="errorType" t="i"/>
+    <k n="rwOffset" t="i"/>
+    <k n="subType" t="i"/>
+  </s>
+</rvStructures>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -949,6 +1026,9 @@
   <we:bindings/>
   <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
   <we:extLst>
+    <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{D87F86FE-615C-45B5-9D79-34F1136793EB}">
+      <we:containsCustomFunctions/>
+    </a:ext>
     <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{7C84B067-C214-45C3-A712-C9D94CD141B2}">
       <we:customFunctionIdList>
         <we:customFunctionIds>_xldudf_LABS_GENERATIVEAI</we:customFunctionIds>
@@ -979,12 +1059,12 @@
         <v>5</v>
       </c>
       <c r="D1" s="4"/>
-      <c r="E1" s="35" t="s">
+      <c r="E1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="J1" s="36" t="s">
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="J1" s="35" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1232,10 +1312,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28BDC360-8D84-479A-A154-556548DB1B28}">
-  <dimension ref="B1:K37"/>
+  <dimension ref="B1:S37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="I20" sqref="I20:O20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1247,21 +1327,21 @@
     <col min="10" max="10" width="10.09765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:19" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D1" s="4"/>
-      <c r="E1" s="35" t="s">
+      <c r="E1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="J1" s="36" t="s">
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="J1" s="35" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="2:11" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:19" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1"/>
       <c r="C2" s="22" t="s">
         <v>6</v>
@@ -1277,7 +1357,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1" cm="1">
         <f t="array" ref="B3:B24">ROW(C3:C24)</f>
         <v>3</v>
@@ -1297,7 +1377,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="1">
         <v>4</v>
       </c>
@@ -1315,7 +1395,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <v>5</v>
       </c>
@@ -1333,7 +1413,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
         <v>6</v>
       </c>
@@ -1350,8 +1430,11 @@
       <c r="G6" s="7">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="S6" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <v>7</v>
       </c>
@@ -1368,8 +1451,11 @@
       <c r="G7" s="34">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="S7" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
         <v>8</v>
       </c>
@@ -1386,8 +1472,11 @@
       <c r="G8" s="18">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="S8" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="2:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
         <v>9</v>
       </c>
@@ -1404,8 +1493,11 @@
       <c r="G9" s="18">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="S9" s="1">
+        <v>45509</v>
+      </c>
+    </row>
+    <row r="10" spans="2:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B10" s="1">
         <v>10</v>
       </c>
@@ -1422,8 +1514,11 @@
       <c r="G10" s="18">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="S10" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="2:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B11" s="1">
         <v>11</v>
       </c>
@@ -1440,8 +1535,11 @@
       <c r="G11" s="7">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="S11" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B12" s="1">
         <v>12</v>
       </c>
@@ -1457,32 +1555,44 @@
       <c r="G12" s="10">
         <v>2</v>
       </c>
-    </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="S12">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B13" s="1">
         <v>13</v>
       </c>
       <c r="C13" s="30" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="S13" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B14" s="1">
         <v>14</v>
       </c>
       <c r="C14" s="31">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="S14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B15" s="1">
         <v>15</v>
       </c>
       <c r="C15" s="27">
         <v>45553</v>
       </c>
-    </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="S15">
+        <v>45517</v>
+      </c>
+    </row>
+    <row r="16" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B16" s="1">
         <v>16</v>
       </c>
@@ -1508,20 +1618,35 @@
         <f ca="1"/>
         <v>10</v>
       </c>
-      <c r="I16" cm="1">
-        <f t="array" aca="1" ref="I16:I37" ca="1">_xlfn.SCAN(, C3:C24, _xleta.MAX)</f>
-        <v>45493</v>
-      </c>
-      <c r="J16" s="37" cm="1">
+      <c r="I16" t="e" cm="1" vm="1">
+        <f t="array" aca="1" ref="I16" ca="1">_xlfn.SCAN(, C3:C24, _xleta.MAX)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="J16" s="36" cm="1">
         <f t="array" aca="1" ref="J16:J37" ca="1">C3:C24</f>
         <v>45493</v>
       </c>
       <c r="K16" cm="1">
-        <f t="array" aca="1" ref="K16" ca="1">_xlfn.XLOOKUP(B3, _b / (_a &lt; 99), _a, , 1)</f>
+        <f t="array" ref="K16:K37">_b/(_a11 &lt;99)</f>
+        <v>3</v>
+      </c>
+      <c r="M16" cm="1">
+        <f t="array" ref="M16:M37">_b</f>
+        <v>3</v>
+      </c>
+      <c r="N16" cm="1">
+        <f t="array" ref="N16:N37">_a11</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="O16" cm="1">
+        <f t="array" ref="O16:O37">_xlfn.XLOOKUP(_xlfn.ANCHORARRAY(M16),_xlfn.ANCHORARRAY(M16)/(_xlfn.ANCHORARRAY(N16)&lt;99),_xlfn.ANCHORARRAY(N16),,1)</f>
+        <v>0</v>
+      </c>
+      <c r="S16" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B17" s="1">
         <v>17</v>
       </c>
@@ -1540,20 +1665,27 @@
         <f ca="1"/>
         <v>8</v>
       </c>
-      <c r="I17">
-        <f ca="1"/>
-        <v>45493</v>
-      </c>
       <c r="J17" t="str">
         <f ca="1"/>
         <v>A</v>
       </c>
-      <c r="K17" cm="1">
-        <f t="array" aca="1" ref="K17" ca="1">_xlfn.XLOOKUP(B4, _b / (_a &lt; 99), _a, , 1)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K17" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M17">
+        <v>4</v>
+      </c>
+      <c r="N17" t="str">
+        <v>A</v>
+      </c>
+      <c r="O17">
+        <v>10</v>
+      </c>
+      <c r="S17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B18" s="1">
         <v>18</v>
       </c>
@@ -1572,20 +1704,27 @@
         <f ca="1"/>
         <v>8</v>
       </c>
-      <c r="I18">
-        <f ca="1"/>
-        <v>45493</v>
-      </c>
       <c r="J18">
         <f ca="1"/>
         <v>10</v>
       </c>
-      <c r="K18" cm="1">
-        <f t="array" aca="1" ref="K18" ca="1">_xlfn.XLOOKUP(B5, _b / (_a &lt; 99), _a, , 1)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K18">
+        <v>5</v>
+      </c>
+      <c r="M18">
+        <v>5</v>
+      </c>
+      <c r="N18">
+        <v>10</v>
+      </c>
+      <c r="O18">
+        <v>10</v>
+      </c>
+      <c r="S18">
+        <v>45553</v>
+      </c>
+    </row>
+    <row r="19" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B19" s="1">
         <v>19</v>
       </c>
@@ -1604,20 +1743,27 @@
         <f ca="1"/>
         <v>2</v>
       </c>
-      <c r="I19">
+      <c r="J19">
         <f ca="1"/>
         <v>45509</v>
       </c>
-      <c r="J19">
-        <f ca="1"/>
+      <c r="K19" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M19">
+        <v>6</v>
+      </c>
+      <c r="N19">
         <v>45509</v>
       </c>
-      <c r="K19" cm="1">
-        <f t="array" aca="1" ref="K19" ca="1">_xlfn.XLOOKUP(B6, _b / (_a &lt; 99), _a, , 1)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="O19">
+        <v>8</v>
+      </c>
+      <c r="S19" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B20" s="1">
         <v>20</v>
       </c>
@@ -1636,20 +1782,27 @@
         <f ca="1"/>
         <v>1</v>
       </c>
-      <c r="I20">
-        <f ca="1"/>
-        <v>45509</v>
-      </c>
       <c r="J20" t="str">
         <f ca="1"/>
         <v>C</v>
       </c>
-      <c r="K20" cm="1">
-        <f t="array" aca="1" ref="K20" ca="1">_xlfn.XLOOKUP(B7, _b / (_a &lt; 99), _a, , 1)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K20" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M20">
+        <v>7</v>
+      </c>
+      <c r="N20" t="str">
+        <v>C</v>
+      </c>
+      <c r="O20">
+        <v>8</v>
+      </c>
+      <c r="S20" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B21" s="1">
         <v>21</v>
       </c>
@@ -1668,20 +1821,27 @@
         <f ca="1"/>
         <v>5</v>
       </c>
-      <c r="I21">
-        <f ca="1"/>
-        <v>45509</v>
-      </c>
       <c r="J21" t="str">
         <f ca="1"/>
         <v>B</v>
       </c>
-      <c r="K21" cm="1">
-        <f t="array" aca="1" ref="K21" ca="1">_xlfn.XLOOKUP(B8, _b / (_a &lt; 99), _a, , 1)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K21" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M21">
+        <v>8</v>
+      </c>
+      <c r="N21" t="str">
+        <v>B</v>
+      </c>
+      <c r="O21">
+        <v>8</v>
+      </c>
+      <c r="S21" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B22" s="1">
         <v>22</v>
       </c>
@@ -1700,20 +1860,27 @@
         <f ca="1"/>
         <v>5</v>
       </c>
-      <c r="I22">
-        <f ca="1"/>
-        <v>45509</v>
-      </c>
       <c r="J22">
         <f ca="1"/>
         <v>8</v>
       </c>
-      <c r="K22" cm="1">
-        <f t="array" aca="1" ref="K22" ca="1">_xlfn.XLOOKUP(B9, _b / (_a &lt; 99), _a, , 1)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K22">
+        <v>9</v>
+      </c>
+      <c r="M22">
+        <v>9</v>
+      </c>
+      <c r="N22">
+        <v>8</v>
+      </c>
+      <c r="O22">
+        <v>8</v>
+      </c>
+      <c r="S22">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B23" s="1">
         <v>23</v>
       </c>
@@ -1732,20 +1899,27 @@
         <f ca="1"/>
         <v>5</v>
       </c>
-      <c r="I23">
-        <f ca="1"/>
-        <v>45509</v>
-      </c>
       <c r="J23" t="str">
         <f ca="1"/>
         <v>A</v>
       </c>
-      <c r="K23" cm="1">
-        <f t="array" aca="1" ref="K23" ca="1">_xlfn.XLOOKUP(B10, _b / (_a &lt; 99), _a, , 1)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K23" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M23">
+        <v>10</v>
+      </c>
+      <c r="N23" t="str">
+        <v>A</v>
+      </c>
+      <c r="O23">
+        <v>2</v>
+      </c>
+      <c r="S23">
+        <v>45566</v>
+      </c>
+    </row>
+    <row r="24" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B24" s="1">
         <v>24</v>
       </c>
@@ -1764,20 +1938,27 @@
         <f ca="1"/>
         <v>1</v>
       </c>
-      <c r="I24">
-        <f ca="1"/>
-        <v>45509</v>
-      </c>
       <c r="J24">
         <f ca="1"/>
         <v>2</v>
       </c>
-      <c r="K24" cm="1">
-        <f t="array" aca="1" ref="K24" ca="1">_xlfn.XLOOKUP(B11, _b / (_a &lt; 99), _a, , 1)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K24">
+        <v>11</v>
+      </c>
+      <c r="M24">
+        <v>11</v>
+      </c>
+      <c r="N24">
+        <v>2</v>
+      </c>
+      <c r="O24">
+        <v>2</v>
+      </c>
+      <c r="S24" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="2:19" x14ac:dyDescent="0.25">
       <c r="E25" s="5">
         <f ca="1"/>
         <v>45566</v>
@@ -1790,185 +1971,246 @@
         <f ca="1"/>
         <v>2</v>
       </c>
-      <c r="I25">
+      <c r="J25">
         <f ca="1"/>
         <v>45517</v>
       </c>
-      <c r="J25">
-        <f ca="1"/>
+      <c r="K25" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M25">
+        <v>12</v>
+      </c>
+      <c r="N25">
         <v>45517</v>
       </c>
-      <c r="K25" cm="1">
-        <f t="array" aca="1" ref="K25" ca="1">_xlfn.XLOOKUP(B12, _b / (_a &lt; 99), _a, , 1)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="I26">
-        <f ca="1"/>
-        <v>45517</v>
-      </c>
+      <c r="O25">
+        <v>1</v>
+      </c>
+      <c r="S25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="2:19" x14ac:dyDescent="0.25">
       <c r="J26" t="str">
         <f ca="1"/>
         <v>B</v>
       </c>
-      <c r="K26" cm="1">
-        <f t="array" aca="1" ref="K26" ca="1">_xlfn.XLOOKUP(B13, _b / (_a &lt; 99), _a, , 1)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="I27">
-        <f ca="1"/>
-        <v>45517</v>
-      </c>
+      <c r="K26" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M26">
+        <v>13</v>
+      </c>
+      <c r="N26" t="str">
+        <v>B</v>
+      </c>
+      <c r="O26">
+        <v>1</v>
+      </c>
+      <c r="S26" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="2:19" x14ac:dyDescent="0.25">
       <c r="J27">
         <f ca="1"/>
         <v>1</v>
       </c>
-      <c r="K27" cm="1">
-        <f t="array" aca="1" ref="K27" ca="1">_xlfn.XLOOKUP(B14, _b / (_a &lt; 99), _a, , 1)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="I28">
+      <c r="K27">
+        <v>14</v>
+      </c>
+      <c r="M27">
+        <v>14</v>
+      </c>
+      <c r="N27">
+        <v>1</v>
+      </c>
+      <c r="O27">
+        <v>1</v>
+      </c>
+      <c r="S27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="J28">
         <f ca="1"/>
         <v>45553</v>
       </c>
-      <c r="J28">
-        <f ca="1"/>
+      <c r="K28" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M28">
+        <v>15</v>
+      </c>
+      <c r="N28">
         <v>45553</v>
       </c>
-      <c r="K28" cm="1">
-        <f t="array" aca="1" ref="K28" ca="1">_xlfn.XLOOKUP(B15, _b / (_a &lt; 99), _a, , 1)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="I29">
-        <f ca="1"/>
-        <v>45553</v>
-      </c>
+      <c r="O28">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="2:19" x14ac:dyDescent="0.25">
       <c r="J29" t="str">
         <f ca="1"/>
         <v>A</v>
       </c>
-      <c r="K29" cm="1">
-        <f t="array" aca="1" ref="K29" ca="1">_xlfn.XLOOKUP(B16, _b / (_a &lt; 99), _a, , 1)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="I30">
-        <f ca="1"/>
-        <v>45553</v>
-      </c>
+      <c r="K29" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M29">
+        <v>16</v>
+      </c>
+      <c r="N29" t="str">
+        <v>A</v>
+      </c>
+      <c r="O29">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="2:19" x14ac:dyDescent="0.25">
       <c r="J30" t="str">
         <f ca="1"/>
         <v>B</v>
       </c>
-      <c r="K30" cm="1">
-        <f t="array" aca="1" ref="K30" ca="1">_xlfn.XLOOKUP(B17, _b / (_a &lt; 99), _a, , 1)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="I31">
-        <f ca="1"/>
-        <v>45553</v>
-      </c>
+      <c r="K30" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M30">
+        <v>17</v>
+      </c>
+      <c r="N30" t="str">
+        <v>B</v>
+      </c>
+      <c r="O30">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="2:19" x14ac:dyDescent="0.25">
       <c r="J31" t="str">
         <f ca="1"/>
         <v>C</v>
       </c>
-      <c r="K31" cm="1">
-        <f t="array" aca="1" ref="K31" ca="1">_xlfn.XLOOKUP(B18, _b / (_a &lt; 99), _a, , 1)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="I32">
-        <f ca="1"/>
-        <v>45553</v>
-      </c>
+      <c r="K31" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M31">
+        <v>18</v>
+      </c>
+      <c r="N31" t="str">
+        <v>C</v>
+      </c>
+      <c r="O31">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="2:19" x14ac:dyDescent="0.25">
       <c r="J32">
         <f ca="1"/>
         <v>5</v>
       </c>
-      <c r="K32" cm="1">
-        <f t="array" aca="1" ref="K32" ca="1">_xlfn.XLOOKUP(B19, _b / (_a &lt; 99), _a, , 1)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="9:11" x14ac:dyDescent="0.25">
-      <c r="I33">
+      <c r="K32">
+        <v>19</v>
+      </c>
+      <c r="M32">
+        <v>19</v>
+      </c>
+      <c r="N32">
+        <v>5</v>
+      </c>
+      <c r="O32">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="10:15" x14ac:dyDescent="0.25">
+      <c r="J33">
         <f ca="1"/>
         <v>45566</v>
       </c>
-      <c r="J33">
-        <f ca="1"/>
+      <c r="K33" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M33">
+        <v>20</v>
+      </c>
+      <c r="N33">
         <v>45566</v>
       </c>
-      <c r="K33" cm="1">
-        <f t="array" aca="1" ref="K33" ca="1">_xlfn.XLOOKUP(B20, _b / (_a &lt; 99), _a, , 1)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="9:11" x14ac:dyDescent="0.25">
-      <c r="I34">
-        <f ca="1"/>
-        <v>45566</v>
-      </c>
+      <c r="O33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="10:15" x14ac:dyDescent="0.25">
       <c r="J34" t="str">
         <f ca="1"/>
         <v>A</v>
       </c>
-      <c r="K34" cm="1">
-        <f t="array" aca="1" ref="K34" ca="1">_xlfn.XLOOKUP(B21, _b / (_a &lt; 99), _a, , 1)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="9:11" x14ac:dyDescent="0.25">
-      <c r="I35">
-        <f ca="1"/>
-        <v>45566</v>
-      </c>
+      <c r="K34" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M34">
+        <v>21</v>
+      </c>
+      <c r="N34" t="str">
+        <v>A</v>
+      </c>
+      <c r="O34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="10:15" x14ac:dyDescent="0.25">
       <c r="J35">
         <f ca="1"/>
         <v>1</v>
       </c>
-      <c r="K35" cm="1">
-        <f t="array" aca="1" ref="K35" ca="1">_xlfn.XLOOKUP(B22, _b / (_a &lt; 99), _a, , 1)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="9:11" x14ac:dyDescent="0.25">
-      <c r="I36">
-        <f ca="1"/>
-        <v>45566</v>
-      </c>
+      <c r="K35">
+        <v>22</v>
+      </c>
+      <c r="M35">
+        <v>22</v>
+      </c>
+      <c r="N35">
+        <v>1</v>
+      </c>
+      <c r="O35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="10:15" x14ac:dyDescent="0.25">
       <c r="J36" t="str">
         <f ca="1"/>
         <v>B</v>
       </c>
-      <c r="K36" cm="1">
-        <f t="array" aca="1" ref="K36" ca="1">_xlfn.XLOOKUP(B23, _b / (_a &lt; 99), _a, , 1)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="9:11" x14ac:dyDescent="0.25">
-      <c r="I37">
-        <f ca="1"/>
-        <v>45566</v>
-      </c>
+      <c r="K36" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M36">
+        <v>23</v>
+      </c>
+      <c r="N36" t="str">
+        <v>B</v>
+      </c>
+      <c r="O36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="10:15" x14ac:dyDescent="0.25">
       <c r="J37">
         <f ca="1"/>
         <v>2</v>
       </c>
-      <c r="K37" cm="1">
-        <f t="array" aca="1" ref="K37" ca="1">_xlfn.XLOOKUP(B24, _b / (_a &lt; 99), _a, , 1)</f>
-        <v>0</v>
+      <c r="K37">
+        <v>24</v>
+      </c>
+      <c r="M37">
+        <v>24</v>
+      </c>
+      <c r="N37">
+        <v>2</v>
+      </c>
+      <c r="O37">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>